<commit_message>
more files. This version still shows a mismatch with MRI triggers. Must understand what is causing it. Task lasts around 4 seconds longer.
</commit_message>
<xml_diff>
--- a/supp/events/sub-SRM_task-videorating_run-1_event.xlsx
+++ b/supp/events/sub-SRM_task-videorating_run-1_event.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="83" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="211" uniqueCount="6">
   <si>
     <t>TR</t>
   </si>
@@ -28,6 +28,9 @@
   </si>
   <si>
     <t>SimTR</t>
+  </si>
+  <si>
+    <t>TrueTR</t>
   </si>
 </sst>
 </file>
@@ -101,41 +104,41 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="0">
-        <v>2.0003874000000001</v>
+        <v>0.0021868999999999999</v>
       </c>
       <c r="C2" s="1">
-        <v>45680.517233194769</v>
+        <v>45686.686356194259</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="0">
-        <v>4.0015333000000002</v>
+        <v>3.8212373999999998</v>
       </c>
       <c r="C3" s="1">
-        <v>45680.517256351006</v>
+        <v>45686.686400229286</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B4" s="0">
-        <v>6.0026324000000004</v>
+        <v>4.0191001000000002</v>
       </c>
       <c r="C4" s="1">
-        <v>45680.517279512962</v>
+        <v>45686.68640256011</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>4</v>
@@ -143,27 +146,27 @@
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5" s="0">
-        <v>8.0030882000000005</v>
+        <v>5.0207367999999999</v>
       </c>
       <c r="C5" s="1">
-        <v>45680.517302666252</v>
+        <v>45686.686414133357</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B6" s="0">
-        <v>10.0025525</v>
+        <v>6.0196991000000004</v>
       </c>
       <c r="C6" s="1">
-        <v>45680.517325806562</v>
+        <v>45686.686425693057</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>4</v>
@@ -171,27 +174,27 @@
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B7" s="0">
-        <v>12.0025105</v>
+        <v>7.5409136999999999</v>
       </c>
       <c r="C7" s="1">
-        <v>45680.517348954352</v>
+        <v>45686.686443273204</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B8" s="0">
-        <v>14.0021977</v>
+        <v>8.0368031999999996</v>
       </c>
       <c r="C8" s="1">
-        <v>45680.517372099144</v>
+        <v>45686.686449009678</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>4</v>
@@ -199,13 +202,13 @@
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B9" s="0">
-        <v>16.003154899999998</v>
+        <v>10.0511208</v>
       </c>
       <c r="C9" s="1">
-        <v>45680.517395260154</v>
+        <v>45686.68647232365</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>4</v>
@@ -213,27 +216,27 @@
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B10" s="0">
-        <v>18.033983299999999</v>
+        <v>10.056268899999999</v>
       </c>
       <c r="C10" s="1">
-        <v>45680.517418762814</v>
+        <v>45686.686472382593</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B11" s="0">
-        <v>20.0005755</v>
+        <v>12.005111899999999</v>
       </c>
       <c r="C11" s="1">
-        <v>45680.517441525735</v>
+        <v>45686.686494941023</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>4</v>
@@ -241,27 +244,27 @@
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B12" s="0">
-        <v>22.017344999999999</v>
+        <v>12.5400432</v>
       </c>
       <c r="C12" s="1">
-        <v>45680.517464867662</v>
+        <v>45686.686501129057</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B13" s="0">
-        <v>24.000166100000001</v>
+        <v>14.0394325</v>
       </c>
       <c r="C13" s="1">
-        <v>45680.517487817961</v>
+        <v>45686.686518486342</v>
       </c>
       <c r="D13" s="0" t="s">
         <v>4</v>
@@ -269,41 +272,41 @@
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B14" s="0">
-        <v>26.000073</v>
+        <v>15.021493700000001</v>
       </c>
       <c r="C14" s="1">
-        <v>45680.517510963808</v>
+        <v>45686.686529850544</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B15" s="0">
-        <v>28.0001426</v>
+        <v>15.072672600000001</v>
       </c>
       <c r="C15" s="1">
-        <v>45680.517534113227</v>
+        <v>45686.686530442712</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B16" s="0">
-        <v>30.000051200000001</v>
+        <v>16.0204369</v>
       </c>
       <c r="C16" s="1">
-        <v>45680.5175572601</v>
+        <v>45686.686541413197</v>
       </c>
       <c r="D16" s="0" t="s">
         <v>4</v>
@@ -311,27 +314,27 @@
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B17" s="0">
-        <v>32.000081899999998</v>
+        <v>17.5398979</v>
       </c>
       <c r="C17" s="1">
-        <v>45680.51758040845</v>
+        <v>45686.686558997913</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B18" s="0">
-        <v>34.001155699999998</v>
+        <v>18.020530999999998</v>
       </c>
       <c r="C18" s="1">
-        <v>45680.517603570879</v>
+        <v>45686.686564561111</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>4</v>
@@ -339,13 +342,13 @@
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B19" s="0">
-        <v>36.0010677</v>
+        <v>20.021532400000002</v>
       </c>
       <c r="C19" s="1">
-        <v>45680.517626715766</v>
+        <v>45686.686587720877</v>
       </c>
       <c r="D19" s="0" t="s">
         <v>4</v>
@@ -353,41 +356,41 @@
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="B20" s="0">
-        <v>38.001191300000002</v>
+        <v>20.023060699999998</v>
       </c>
       <c r="C20" s="1">
-        <v>45680.517649866488</v>
+        <v>45686.686587737437</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B21" s="0">
-        <v>40.003782100000002</v>
+        <v>20.0711206</v>
       </c>
       <c r="C21" s="1">
-        <v>45680.517673044364</v>
+        <v>45686.686588294811</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="B22" s="0">
-        <v>42.003398400000002</v>
+        <v>22.039170500000001</v>
       </c>
       <c r="C22" s="1">
-        <v>45680.517696186631</v>
+        <v>45686.68661107299</v>
       </c>
       <c r="D22" s="0" t="s">
         <v>4</v>
@@ -395,41 +398,41 @@
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="B23" s="0">
-        <v>44.003234999999997</v>
+        <v>22.539384500000001</v>
       </c>
       <c r="C23" s="1">
-        <v>45680.51771933437</v>
+        <v>45686.686616864034</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B24" s="0">
-        <v>46.002333100000001</v>
+        <v>22.555964299999999</v>
       </c>
       <c r="C24" s="1">
-        <v>45680.517742470453</v>
+        <v>45686.686617054584</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B25" s="0">
-        <v>48.034762700000002</v>
+        <v>24.020783099999999</v>
       </c>
       <c r="C25" s="1">
-        <v>45680.51776599422</v>
+        <v>45686.686634009166</v>
       </c>
       <c r="D25" s="0" t="s">
         <v>4</v>
@@ -437,27 +440,27 @@
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="B26" s="0">
-        <v>50.003669799999997</v>
+        <v>25.0259578</v>
       </c>
       <c r="C26" s="1">
-        <v>45680.517788782374</v>
+        <v>45686.686645642294</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="B27" s="0">
-        <v>52.003602200000003</v>
+        <v>26.002044300000001</v>
       </c>
       <c r="C27" s="1">
-        <v>45680.517811931146</v>
+        <v>45686.686656942671</v>
       </c>
       <c r="D27" s="0" t="s">
         <v>4</v>
@@ -465,41 +468,41 @@
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="B28" s="0">
-        <v>54.000028999999998</v>
+        <v>27.515249600000001</v>
       </c>
       <c r="C28" s="1">
-        <v>45680.517835037506</v>
+        <v>45686.686674453755</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="B29" s="0">
-        <v>56.000087100000002</v>
+        <v>27.549562399999999</v>
       </c>
       <c r="C29" s="1">
-        <v>45680.517858186169</v>
+        <v>45686.686674851604</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="B30" s="0">
-        <v>58.000038799999999</v>
+        <v>28.00001</v>
       </c>
       <c r="C30" s="1">
-        <v>45680.517881333726</v>
+        <v>45686.686680063627</v>
       </c>
       <c r="D30" s="0" t="s">
         <v>4</v>
@@ -507,13 +510,13 @@
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="B31" s="0">
-        <v>60.000065999999997</v>
+        <v>30.000041499999998</v>
       </c>
       <c r="C31" s="1">
-        <v>45680.517904482294</v>
+        <v>45686.686703212843</v>
       </c>
       <c r="D31" s="0" t="s">
         <v>4</v>
@@ -521,41 +524,41 @@
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="B32" s="0">
-        <v>62.000042899999997</v>
+        <v>30.042865899999999</v>
       </c>
       <c r="C32" s="1">
-        <v>45680.51792763007</v>
+        <v>45686.686703707986</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="B33" s="0">
-        <v>64.002157199999999</v>
+        <v>30.058609300000001</v>
       </c>
       <c r="C33" s="1">
-        <v>45680.517950803136</v>
+        <v>45686.686703891108</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="B34" s="0">
-        <v>66.002211700000004</v>
+        <v>32.000104999999998</v>
       </c>
       <c r="C34" s="1">
-        <v>45680.517973954098</v>
+        <v>45686.686726361862</v>
       </c>
       <c r="D34" s="0" t="s">
         <v>4</v>
@@ -563,41 +566,41 @@
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="B35" s="0">
-        <v>68.002237100000002</v>
+        <v>32.538333899999998</v>
       </c>
       <c r="C35" s="1">
-        <v>45680.517997099443</v>
+        <v>45686.686732590962</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="B36" s="0">
-        <v>70.002120899999994</v>
+        <v>32.552061600000002</v>
       </c>
       <c r="C36" s="1">
-        <v>45680.518020246425</v>
+        <v>45686.686732750059</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="B37" s="0">
-        <v>72.003858800000003</v>
+        <v>34.000054400000003</v>
       </c>
       <c r="C37" s="1">
-        <v>45680.518043414406</v>
+        <v>45686.686749510925</v>
       </c>
       <c r="D37" s="0" t="s">
         <v>4</v>
@@ -605,13 +608,13 @@
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="B38" s="0">
-        <v>74.004565700000001</v>
+        <v>36.4229828</v>
       </c>
       <c r="C38" s="1">
-        <v>45680.518066573379</v>
+        <v>45686.686777552648</v>
       </c>
       <c r="D38" s="0" t="s">
         <v>4</v>
@@ -619,203 +622,283 @@
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B39" s="0">
-        <v>0</v>
-      </c>
-      <c r="C39" s="1"/>
-      <c r="D39" s="0"/>
+        <v>36.424269199999998</v>
+      </c>
+      <c r="C39" s="1">
+        <v>45686.686777565548</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="B40" s="0">
-        <v>0</v>
-      </c>
-      <c r="C40" s="1"/>
-      <c r="D40" s="0"/>
+        <v>37.536952599999999</v>
+      </c>
+      <c r="C40" s="1">
+        <v>45686.686790445543</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="B41" s="0">
-        <v>0</v>
-      </c>
-      <c r="C41" s="1"/>
-      <c r="D41" s="0"/>
+        <v>37.570059499999999</v>
+      </c>
+      <c r="C41" s="1">
+        <v>45686.686790829408</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="B42" s="0">
-        <v>0</v>
-      </c>
-      <c r="C42" s="1"/>
-      <c r="D42" s="0"/>
+        <v>38.0031319</v>
+      </c>
+      <c r="C42" s="1">
+        <v>45686.686795841153</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="B43" s="0">
-        <v>0</v>
-      </c>
-      <c r="C43" s="1"/>
-      <c r="D43" s="0"/>
+        <v>40.003137299999999</v>
+      </c>
+      <c r="C43" s="1">
+        <v>45686.6868189897</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="0">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B44" s="0">
-        <v>0</v>
-      </c>
-      <c r="C44" s="1"/>
-      <c r="D44" s="0"/>
+        <v>40.037225399999997</v>
+      </c>
+      <c r="C44" s="1">
+        <v>45686.686819385905</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="B45" s="0">
-        <v>0</v>
-      </c>
-      <c r="C45" s="1"/>
-      <c r="D45" s="0"/>
+        <v>40.070220499999998</v>
+      </c>
+      <c r="C45" s="1">
+        <v>45686.686819765535</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="0">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B46" s="0">
-        <v>0</v>
-      </c>
-      <c r="C46" s="1"/>
-      <c r="D46" s="0"/>
+        <v>42.003271300000002</v>
+      </c>
+      <c r="C46" s="1">
+        <v>45686.686842138864</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="0">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="B47" s="0">
-        <v>0</v>
-      </c>
-      <c r="C47" s="1"/>
-      <c r="D47" s="0"/>
+        <v>42.536633700000003</v>
+      </c>
+      <c r="C47" s="1">
+        <v>45686.68684831178</v>
+      </c>
+      <c r="D47" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="0">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="B48" s="0">
-        <v>0</v>
-      </c>
-      <c r="C48" s="1"/>
-      <c r="D48" s="0"/>
+        <v>42.570053799999997</v>
+      </c>
+      <c r="C48" s="1">
+        <v>45686.686848698773</v>
+      </c>
+      <c r="D48" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="0">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="B49" s="0">
-        <v>0</v>
-      </c>
-      <c r="C49" s="1"/>
-      <c r="D49" s="0"/>
+        <v>44.004962300000003</v>
+      </c>
+      <c r="C49" s="1">
+        <v>45686.686865307573</v>
+      </c>
+      <c r="D49" s="0" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="0">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="B50" s="0">
-        <v>0</v>
-      </c>
-      <c r="C50" s="1"/>
-      <c r="D50" s="0"/>
+        <v>45.0381134</v>
+      </c>
+      <c r="C50" s="1">
+        <v>45686.686877263914</v>
+      </c>
+      <c r="D50" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="0">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="B51" s="0">
-        <v>0</v>
-      </c>
-      <c r="C51" s="1"/>
-      <c r="D51" s="0"/>
+        <v>45.072978999999997</v>
+      </c>
+      <c r="C51" s="1">
+        <v>45686.686877668719</v>
+      </c>
+      <c r="D51" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="0">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="B52" s="0">
-        <v>0</v>
-      </c>
-      <c r="C52" s="1"/>
-      <c r="D52" s="0"/>
+        <v>46.004399599999999</v>
+      </c>
+      <c r="C52" s="1">
+        <v>45686.686888449185</v>
+      </c>
+      <c r="D52" s="0" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="0">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="B53" s="0">
-        <v>0</v>
-      </c>
-      <c r="C53" s="1"/>
-      <c r="D53" s="0"/>
+        <v>47.538185900000002</v>
+      </c>
+      <c r="C53" s="1">
+        <v>45686.686906199931</v>
+      </c>
+      <c r="D53" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="0">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="B54" s="0">
-        <v>0</v>
-      </c>
-      <c r="C54" s="1"/>
-      <c r="D54" s="0"/>
+        <v>47.571886999999997</v>
+      </c>
+      <c r="C54" s="1">
+        <v>45686.686906590243</v>
+      </c>
+      <c r="D54" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="0">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B55" s="0">
-        <v>0</v>
-      </c>
-      <c r="C55" s="1"/>
-      <c r="D55" s="0"/>
+        <v>48.003859499999997</v>
+      </c>
+      <c r="C55" s="1">
+        <v>45686.686911590587</v>
+      </c>
+      <c r="D55" s="0" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="0">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="B56" s="0">
-        <v>0</v>
-      </c>
-      <c r="C56" s="1"/>
-      <c r="D56" s="0"/>
+        <v>50.003642800000002</v>
+      </c>
+      <c r="C56" s="1">
+        <v>45686.686934736295</v>
+      </c>
+      <c r="D56" s="0" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="0">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="B57" s="0">
-        <v>0</v>
-      </c>
-      <c r="C57" s="1"/>
-      <c r="D57" s="0"/>
+        <v>50.070648200000001</v>
+      </c>
+      <c r="C57" s="1">
+        <v>45686.686935511236</v>
+      </c>
+      <c r="D57" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="0">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="B58" s="0">
-        <v>0</v>
-      </c>
-      <c r="C58" s="1"/>
-      <c r="D58" s="0"/>
+        <v>52.003482599999998</v>
+      </c>
+      <c r="C58" s="1">
+        <v>45686.686957881626</v>
+      </c>
+      <c r="D58" s="0" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="0">

</xml_diff>